<commit_message>
snapshot and nicolas comments
</commit_message>
<xml_diff>
--- a/output_validation/01_dimension_percentage.xlsx
+++ b/output_validation/01_dimension_percentage.xlsx
@@ -25,6 +25,9 @@
     <t>pop_group</t>
   </si>
   <si>
+    <t>Not in need</t>
+  </si>
+  <si>
     <t>access</t>
   </si>
   <si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t>learning condition</t>
-  </si>
-  <si>
-    <t>not falling within the PiN dimensions</t>
   </si>
   <si>
     <t>protected environment</t>
@@ -498,16 +498,16 @@
         <v>19</v>
       </c>
       <c r="C2">
+        <v>0.7106540107189164</v>
+      </c>
+      <c r="D2">
         <v>0.190710457186663</v>
       </c>
-      <c r="D2">
-        <v>0.09531458339445194</v>
-      </c>
       <c r="E2">
+        <v>0.09531458339445195</v>
+      </c>
+      <c r="F2">
         <v>0.00332094869996863</v>
-      </c>
-      <c r="F2">
-        <v>0.7106540107189163</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -521,16 +521,16 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>0.467334059886158</v>
+        <v>0.3290499252879424</v>
       </c>
       <c r="D3">
+        <v>0.4673340598861581</v>
+      </c>
+      <c r="E3">
         <v>0.02351335102101421</v>
       </c>
-      <c r="E3">
-        <v>0.1363377937635116</v>
-      </c>
       <c r="F3">
-        <v>0.3290499252879423</v>
+        <v>0.1363377937635117</v>
       </c>
       <c r="G3">
         <v>0.0437648700413738</v>
@@ -544,16 +544,16 @@
         <v>19</v>
       </c>
       <c r="C4">
+        <v>0.451490579415013</v>
+      </c>
+      <c r="D4">
         <v>0.3029933244222449</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.02115781288198968</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.1668594842488218</v>
-      </c>
-      <c r="F4">
-        <v>0.451490579415013</v>
       </c>
       <c r="G4">
         <v>0.05749879903193069</v>
@@ -567,16 +567,16 @@
         <v>19</v>
       </c>
       <c r="C5">
+        <v>0.2418234127364369</v>
+      </c>
+      <c r="D5">
         <v>0.6520581443625028</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.01366262932702547</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.07739927371974965</v>
-      </c>
-      <c r="F5">
-        <v>0.2418234127364369</v>
       </c>
       <c r="G5">
         <v>0.01505653985428526</v>
@@ -590,16 +590,16 @@
         <v>19</v>
       </c>
       <c r="C6">
+        <v>0.03115927001577109</v>
+      </c>
+      <c r="D6">
         <v>0.8414055018184412</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.006066203886073819</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.01720586734079309</v>
-      </c>
-      <c r="F6">
-        <v>0.03115927001577109</v>
       </c>
       <c r="G6">
         <v>0.1041631569389209</v>
@@ -613,16 +613,16 @@
         <v>19</v>
       </c>
       <c r="C7">
+        <v>0.3453075914522154</v>
+      </c>
+      <c r="D7">
         <v>0.5532912991791453</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.02136518339723263</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.01254642344682841</v>
-      </c>
-      <c r="F7">
-        <v>0.3453075914522154</v>
       </c>
       <c r="G7">
         <v>0.06748950252457825</v>
@@ -636,16 +636,16 @@
         <v>19</v>
       </c>
       <c r="C8">
+        <v>0.6672571779664611</v>
+      </c>
+      <c r="D8">
         <v>0.2367263812424759</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.06125870664438033</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.02324762293162015</v>
-      </c>
-      <c r="F8">
-        <v>0.6672571779664611</v>
       </c>
       <c r="G8">
         <v>0.01151011121506259</v>
@@ -659,16 +659,16 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>0.4386203619332985</v>
+        <v>0.4300183427740319</v>
       </c>
       <c r="D9">
+        <v>0.4386203619332983</v>
+      </c>
+      <c r="E9">
         <v>0.06879676346048313</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
-        <v>0.430018342774032</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0.06256453183218642</v>
@@ -682,19 +682,19 @@
         <v>19</v>
       </c>
       <c r="C10">
+        <v>0.503759477991108</v>
+      </c>
+      <c r="D10">
         <v>0.270105571906739</v>
       </c>
-      <c r="D10">
-        <v>0.06386966279094732</v>
-      </c>
       <c r="E10">
-        <v>0.05680002453431084</v>
+        <v>0.06386966279094733</v>
       </c>
       <c r="F10">
-        <v>0.5037594779911079</v>
+        <v>0.05680002453431085</v>
       </c>
       <c r="G10">
-        <v>0.1054652627768948</v>
+        <v>0.1054652627768949</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -705,16 +705,16 @@
         <v>19</v>
       </c>
       <c r="C11">
-        <v>0.51007849722683</v>
+        <v>0.3042856291533364</v>
       </c>
       <c r="D11">
+        <v>0.5100784972268301</v>
+      </c>
+      <c r="E11">
         <v>0.005852934652471125</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.02119727645262988</v>
-      </c>
-      <c r="F11">
-        <v>0.3042856291533363</v>
       </c>
       <c r="G11">
         <v>0.1585856625147326</v>
@@ -728,16 +728,16 @@
         <v>19</v>
       </c>
       <c r="C12">
+        <v>0.5351307850709578</v>
+      </c>
+      <c r="D12">
         <v>0.4023060687369476</v>
       </c>
-      <c r="D12">
-        <v>0.03702069958023029</v>
-      </c>
       <c r="E12">
+        <v>0.03702069958023028</v>
+      </c>
+      <c r="F12">
         <v>0.0255424466118643</v>
-      </c>
-      <c r="F12">
-        <v>0.5351307850709578</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -751,16 +751,16 @@
         <v>19</v>
       </c>
       <c r="C13">
+        <v>0.1606215520728562</v>
+      </c>
+      <c r="D13">
         <v>0.780119179566651</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.02185734521386637</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.03031483260684526</v>
-      </c>
-      <c r="F13">
-        <v>0.1606215520728562</v>
       </c>
       <c r="G13">
         <v>0.007087090539781185</v>
@@ -810,16 +810,16 @@
         <v>20</v>
       </c>
       <c r="C2">
+        <v>0.3202038642640018</v>
+      </c>
+      <c r="D2">
         <v>0.5997279723345624</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.01887686599956911</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.009269706648321113</v>
-      </c>
-      <c r="F2">
-        <v>0.3202038642640018</v>
       </c>
       <c r="G2">
         <v>0.05192159075354553</v>
@@ -869,16 +869,16 @@
         <v>27</v>
       </c>
       <c r="C2">
+        <v>0.7355010475254173</v>
+      </c>
+      <c r="D2">
         <v>0.2246645324560284</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.02317121176486182</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.01006463778453275</v>
-      </c>
-      <c r="F2">
-        <v>0.7355010475254173</v>
       </c>
       <c r="G2">
         <v>0.006598570469159679</v>
@@ -892,16 +892,16 @@
         <v>27</v>
       </c>
       <c r="C3">
+        <v>0.2881114296960966</v>
+      </c>
+      <c r="D3">
         <v>0.6370232145138697</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.003355230387105165</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.03677214735238916</v>
-      </c>
-      <c r="F3">
-        <v>0.2881114296960966</v>
       </c>
       <c r="G3">
         <v>0.0347379780505395</v>
@@ -915,16 +915,16 @@
         <v>27</v>
       </c>
       <c r="C4">
-        <v>0.3836873839858632</v>
+        <v>0.542864226316311</v>
       </c>
       <c r="D4">
-        <v>0.04386467216042553</v>
+        <v>0.3836873839858633</v>
       </c>
       <c r="E4">
-        <v>0.01396140443210469</v>
+        <v>0.04386467216042554</v>
       </c>
       <c r="F4">
-        <v>0.542864226316311</v>
+        <v>0.0139614044321047</v>
       </c>
       <c r="G4">
         <v>0.01562231310529551</v>
@@ -938,16 +938,16 @@
         <v>27</v>
       </c>
       <c r="C5">
+        <v>0.2957402131124322</v>
+      </c>
+      <c r="D5">
         <v>0.6475361562386643</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.02662675445858609</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.01034372974580771</v>
-      </c>
-      <c r="F5">
-        <v>0.2957402131124322</v>
       </c>
       <c r="G5">
         <v>0.0197531464445096</v>
@@ -961,16 +961,16 @@
         <v>27</v>
       </c>
       <c r="C6">
+        <v>0.2168995155835067</v>
+      </c>
+      <c r="D6">
         <v>0.7067734103739008</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.0479594500977146</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.02380464262637988</v>
-      </c>
-      <c r="F6">
-        <v>0.2168995155835067</v>
       </c>
       <c r="G6">
         <v>0.004562981318497784</v>
@@ -984,16 +984,16 @@
         <v>27</v>
       </c>
       <c r="C7">
+        <v>0.7255237755561456</v>
+      </c>
+      <c r="D7">
         <v>0.2031253855922261</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.03740669864710201</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.0339441402045264</v>
-      </c>
-      <c r="F7">
-        <v>0.7255237755561456</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1007,19 +1007,19 @@
         <v>27</v>
       </c>
       <c r="C8">
+        <v>0.7749837497270198</v>
+      </c>
+      <c r="D8">
         <v>0.2011021168930733</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.01010426870802466</v>
       </c>
-      <c r="E8">
-        <v>0.008707118220853689</v>
-      </c>
       <c r="F8">
-        <v>0.7749837497270196</v>
+        <v>0.008707118220853691</v>
       </c>
       <c r="G8">
-        <v>0.005102746451028844</v>
+        <v>0.005102746451028845</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1030,16 +1030,16 @@
         <v>27</v>
       </c>
       <c r="C9">
+        <v>0.7567306197548092</v>
+      </c>
+      <c r="D9">
         <v>0.1048223149121534</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.07569739695083222</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.06274966838220511</v>
-      </c>
-      <c r="F9">
-        <v>0.7567306197548092</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1053,16 +1053,16 @@
         <v>27</v>
       </c>
       <c r="C10">
+        <v>0.7815722567773472</v>
+      </c>
+      <c r="D10">
         <v>0.2048177817451928</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.0136099614774599</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
       <c r="F10">
-        <v>0.7815722567773472</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1076,16 +1076,16 @@
         <v>27</v>
       </c>
       <c r="C11">
+        <v>0.7738342948998559</v>
+      </c>
+      <c r="D11">
         <v>0.1046527264059715</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.03543814744568882</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.0788805680596739</v>
-      </c>
-      <c r="F11">
-        <v>0.7738342948998559</v>
       </c>
       <c r="G11">
         <v>0.007194263188809723</v>
@@ -1099,16 +1099,16 @@
         <v>27</v>
       </c>
       <c r="C12">
+        <v>0.6759834838293406</v>
+      </c>
+      <c r="D12">
         <v>0.1111364861551428</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.07403526563460644</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.04505024459947984</v>
-      </c>
-      <c r="F12">
-        <v>0.6759834838293406</v>
       </c>
       <c r="G12">
         <v>0.0937945197814303</v>
@@ -1122,16 +1122,16 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>0.4037508980516129</v>
+        <v>0.4619138320502865</v>
       </c>
       <c r="D13">
+        <v>0.403750898051613</v>
+      </c>
+      <c r="E13">
         <v>0.01966706479867863</v>
       </c>
-      <c r="E13">
-        <v>0.07811591978181061</v>
-      </c>
       <c r="F13">
-        <v>0.4619138320502864</v>
+        <v>0.07811591978181062</v>
       </c>
       <c r="G13">
         <v>0.03655228531761142</v>
@@ -1145,19 +1145,19 @@
         <v>27</v>
       </c>
       <c r="C14">
-        <v>0.2580592382461158</v>
+        <v>0.6577904324554799</v>
       </c>
       <c r="D14">
-        <v>0.07780282150174836</v>
+        <v>0.2580592382461159</v>
       </c>
       <c r="E14">
-        <v>0.002059391714946342</v>
+        <v>0.07780282150174837</v>
       </c>
       <c r="F14">
-        <v>0.6577904324554797</v>
+        <v>0.002059391714946343</v>
       </c>
       <c r="G14">
-        <v>0.004288116081709647</v>
+        <v>0.004288116081709648</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1168,16 +1168,16 @@
         <v>27</v>
       </c>
       <c r="C15">
+        <v>0.8174822877535954</v>
+      </c>
+      <c r="D15">
         <v>0.07499063577569208</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.04406802745667497</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.06345904901403755</v>
-      </c>
-      <c r="F15">
-        <v>0.8174822877535954</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1191,19 +1191,19 @@
         <v>27</v>
       </c>
       <c r="C16">
+        <v>0.538121125714962</v>
+      </c>
+      <c r="D16">
         <v>0.3438485809116489</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0.05173825925298021</v>
       </c>
-      <c r="E16">
-        <v>0.05389118409563316</v>
-      </c>
       <c r="F16">
-        <v>0.5381211257149618</v>
+        <v>0.05389118409563317</v>
       </c>
       <c r="G16">
-        <v>0.01240085002477573</v>
+        <v>0.01240085002477574</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1214,16 +1214,16 @@
         <v>27</v>
       </c>
       <c r="C17">
+        <v>0.8548534137558078</v>
+      </c>
+      <c r="D17">
         <v>0.1094267861545242</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.03571980008966798</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
-        <v>0.8548534137558078</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1237,16 +1237,16 @@
         <v>27</v>
       </c>
       <c r="C18">
+        <v>0.9248139239710328</v>
+      </c>
+      <c r="D18">
         <v>0.03634751776327397</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.03292999288485467</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
-        <v>0.9248139239710328</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0.005908565380838581</v>
@@ -1260,16 +1260,16 @@
         <v>27</v>
       </c>
       <c r="C19">
+        <v>0.87123704802994</v>
+      </c>
+      <c r="D19">
         <v>0.08039684079360003</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.04347052377995093</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>0.004895587396509143</v>
-      </c>
-      <c r="F19">
-        <v>0.87123704802994</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1319,16 +1319,16 @@
         <v>28</v>
       </c>
       <c r="C2">
+        <v>0.5993405930558748</v>
+      </c>
+      <c r="D2">
         <v>0.3461159896987495</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.03700134904572487</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.01754206819965072</v>
-      </c>
-      <c r="F2">
-        <v>0.5993405930558748</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1342,16 +1342,16 @@
         <v>28</v>
       </c>
       <c r="C3">
+        <v>0.1643234671516556</v>
+      </c>
+      <c r="D3">
         <v>0.5363990822578679</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.01688281685020779</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.1905420565106229</v>
-      </c>
-      <c r="F3">
-        <v>0.1643234671516556</v>
       </c>
       <c r="G3">
         <v>0.09185257722964593</v>
@@ -1365,16 +1365,16 @@
         <v>28</v>
       </c>
       <c r="C4">
+        <v>0.4917716660792544</v>
+      </c>
+      <c r="D4">
         <v>0.4861326132088599</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0.01567743048028169</v>
-      </c>
-      <c r="F4">
-        <v>0.4917716660792544</v>
       </c>
       <c r="G4">
         <v>0.006418290231603985</v>
@@ -1388,16 +1388,16 @@
         <v>28</v>
       </c>
       <c r="C5">
+        <v>0.4068563174242846</v>
+      </c>
+      <c r="D5">
         <v>0.5296564849408226</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.03816465636136621</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.01414738013903636</v>
-      </c>
-      <c r="F5">
-        <v>0.4068563174242846</v>
       </c>
       <c r="G5">
         <v>0.01117516113449035</v>
@@ -1411,16 +1411,16 @@
         <v>28</v>
       </c>
       <c r="C6">
+        <v>0.07562392814612101</v>
+      </c>
+      <c r="D6">
         <v>0.9193078839006363</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0.005068187953242716</v>
-      </c>
-      <c r="F6">
-        <v>0.07562392814612101</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1434,16 +1434,16 @@
         <v>28</v>
       </c>
       <c r="C7">
+        <v>0.5497172552716943</v>
+      </c>
+      <c r="D7">
         <v>0.3892670239583827</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.06101572076992296</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
-        <v>0.5497172552716943</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1457,16 +1457,16 @@
         <v>28</v>
       </c>
       <c r="C8">
+        <v>0.4732055462978784</v>
+      </c>
+      <c r="D8">
         <v>0.4160086106878902</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.0432878883621454</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.06749795465208604</v>
-      </c>
-      <c r="F8">
-        <v>0.4732055462978784</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1480,16 +1480,16 @@
         <v>28</v>
       </c>
       <c r="C9">
+        <v>0.2802404301971403</v>
+      </c>
+      <c r="D9">
         <v>0.4304411167262168</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.08493390733218803</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.1063556480784028</v>
-      </c>
-      <c r="F9">
-        <v>0.2802404301971403</v>
       </c>
       <c r="G9">
         <v>0.09802889766605188</v>
@@ -1503,16 +1503,16 @@
         <v>28</v>
       </c>
       <c r="C10">
+        <v>0.5337870602633682</v>
+      </c>
+      <c r="D10">
         <v>0.2525549026166085</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.1393912851416745</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.05695902476239229</v>
-      </c>
-      <c r="F10">
-        <v>0.5337870602633682</v>
       </c>
       <c r="G10">
         <v>0.0173077272159565</v>
@@ -1526,16 +1526,16 @@
         <v>28</v>
       </c>
       <c r="C11">
+        <v>0.3287750150324628</v>
+      </c>
+      <c r="D11">
         <v>0.5242081101445487</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.04803177498858425</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.05975679914582763</v>
-      </c>
-      <c r="F11">
-        <v>0.3287750150324628</v>
       </c>
       <c r="G11">
         <v>0.03922830068857657</v>
@@ -1549,16 +1549,16 @@
         <v>28</v>
       </c>
       <c r="C12">
+        <v>0.5928738109452726</v>
+      </c>
+      <c r="D12">
         <v>0.1980015235867318</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.2006406549106493</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.008484010557346435</v>
-      </c>
-      <c r="F12">
-        <v>0.5928738109452726</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1572,19 +1572,19 @@
         <v>28</v>
       </c>
       <c r="C13">
+        <v>0.3666693062507451</v>
+      </c>
+      <c r="D13">
         <v>0.4897918112166131</v>
       </c>
-      <c r="D13">
-        <v>0.06306542781760052</v>
-      </c>
       <c r="E13">
-        <v>0.02701275396855352</v>
+        <v>0.06306542781760054</v>
       </c>
       <c r="F13">
-        <v>0.3666693062507451</v>
+        <v>0.02701275396855353</v>
       </c>
       <c r="G13">
-        <v>0.05346070074648779</v>
+        <v>0.0534607007464878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>